<commit_message>
data format enalarged, error spotted and corrected
</commit_message>
<xml_diff>
--- a/distance_clusters_storages.xlsx
+++ b/distance_clusters_storages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5e6d0361700114d3/Desktop/Optimization Models/Python exercises/DSSC_MO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F8B317B-B317-4ED0-A3E0-7FF187C09283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{4F8B317B-B317-4ED0-A3E0-7FF187C09283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E3FF11E-D155-4EB5-AB53-27015E83393E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D2707CE4-B2AC-407D-AA91-BBE4B442B423}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>C1</t>
   </si>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>S6</t>
-  </si>
-  <si>
-    <t>storage</t>
-  </si>
-  <si>
-    <t>distance</t>
   </si>
   <si>
     <t>3.8</t>
@@ -125,11 +119,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -447,223 +438,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388B7F7A-5715-452C-9501-E28422735903}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="G2" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C6" s="1">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D6" s="1">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
         <v>5.7</v>
       </c>
-      <c r="E3" s="2">
-        <v>16.8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G3" s="2">
-        <v>5.7</v>
-      </c>
-      <c r="H3" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="G6" s="1">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="F4" s="2">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B8" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C8" s="1">
         <v>6.2</v>
       </c>
-      <c r="D5" s="2">
-        <v>6.9</v>
-      </c>
-      <c r="E5" s="2">
-        <v>19.5</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="G5" s="2">
-        <v>3.4</v>
-      </c>
-      <c r="H5" s="2">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5.2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D8" s="1">
         <v>17</v>
       </c>
-      <c r="F6" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G6" s="2">
-        <v>6</v>
-      </c>
-      <c r="H6" s="2">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2.6</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="E8" s="1">
         <v>7</v>
       </c>
-      <c r="E7" s="2">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2">
-        <v>3</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5.7</v>
-      </c>
-      <c r="H7" s="2">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>16.7</v>
-      </c>
-      <c r="F8" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G8" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="H8" s="2">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>17</v>
-      </c>
-      <c r="F9" s="2">
-        <v>7</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F8" s="1">
         <v>5.4</v>
       </c>
-      <c r="H9" s="2">
+      <c r="G8" s="1">
         <v>13.2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A3:A9"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>